<commit_message>
sqlite - union all for modul
</commit_message>
<xml_diff>
--- a/dosyalar/uzfile/Tebligat.xlsx
+++ b/dosyalar/uzfile/Tebligat.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
   <si>
     <t>TEBLİĞ MAZBATASI</t>
   </si>
@@ -139,9 +139,6 @@
   </si>
   <si>
     <t xml:space="preserve">………………………………………………… Buradan katlayınız ………………………………………………… </t>
-  </si>
-  <si>
-    <t>Soruşturma</t>
   </si>
   <si>
     <t>soruşturma No</t>
@@ -512,12 +509,58 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -527,52 +570,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1000,17 +997,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="14" width="9.140625" style="4"/>
-    <col min="15" max="15" width="9.140625" style="50" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" style="51" customWidth="1"/>
-    <col min="17" max="18" width="9.140625" style="4" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="4"/>
+    <col min="15" max="15" width="9.140625" style="50" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" style="51" hidden="1" customWidth="1"/>
+    <col min="17" max="18" width="9.140625" style="4" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1019,20 +1017,20 @@
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="65" t="s">
+      <c r="D1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="3"/>
       <c r="P1" s="51" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q1" s="74">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="54">
         <v>43435</v>
       </c>
     </row>
@@ -1040,47 +1038,47 @@
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="60" t="s">
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="61">
+      <c r="J2" s="59">
         <f>Q1</f>
         <v>43435</v>
       </c>
-      <c r="K2" s="62"/>
+      <c r="K2" s="60"/>
       <c r="P2" s="51" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="62"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="60"/>
       <c r="P3" s="51" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1098,31 +1096,31 @@
       <c r="J4" s="11"/>
       <c r="K4" s="12"/>
       <c r="P4" s="51" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="68"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="63"/>
       <c r="G5" s="13"/>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
       <c r="K5" s="15"/>
       <c r="P5" s="51" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R5" s="4" t="str">
         <f>IF(Q5 = "Kadın","kızı",IF(Q5 = "Erkek","oğlu",))</f>
@@ -1138,15 +1136,15 @@
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
       <c r="F6" s="18"/>
-      <c r="G6" s="69" t="s">
+      <c r="G6" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="63"/>
+      <c r="H6" s="65"/>
       <c r="I6" s="19"/>
       <c r="J6" s="17"/>
       <c r="K6" s="18"/>
       <c r="P6" s="51" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q6" s="53">
         <v>31669</v>
@@ -1161,13 +1159,13 @@
       <c r="D7" s="17"/>
       <c r="E7" s="9"/>
       <c r="F7" s="18"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="63"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="65"/>
       <c r="I7" s="19"/>
       <c r="J7" s="17"/>
       <c r="K7" s="18"/>
       <c r="P7" s="51" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q7" s="4">
         <v>14579213518</v>
@@ -1188,10 +1186,10 @@
       <c r="J8" s="7"/>
       <c r="K8" s="20"/>
       <c r="P8" s="51" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1209,7 +1207,7 @@
       <c r="J9" s="7"/>
       <c r="K9" s="20"/>
       <c r="P9" s="51" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1221,21 +1219,21 @@
       <c r="D10" s="22"/>
       <c r="E10" s="17"/>
       <c r="F10" s="18"/>
-      <c r="G10" s="54" t="s">
+      <c r="G10" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="55" t="str">
+      <c r="H10" s="67" t="str">
         <f>UPPER(Q2)</f>
         <v>MEHMET EROĞLU</v>
       </c>
-      <c r="I10" s="55"/>
+      <c r="I10" s="67"/>
       <c r="J10" s="23"/>
       <c r="K10" s="24"/>
       <c r="P10" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="R10" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="R10" s="4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1247,9 +1245,9 @@
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
       <c r="F11" s="18"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="55"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
       <c r="J11" s="23"/>
       <c r="K11" s="24"/>
     </row>
@@ -1316,13 +1314,13 @@
       <c r="G15" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="70" t="str">
+      <c r="H15" s="68" t="str">
         <f>PROPER(Q8)</f>
         <v>Ambarlı Mah Etinabk Tesisler Yolu Cad. Batman Apt. No:18 Daire 12 Avcılar İstanbul</v>
       </c>
-      <c r="I15" s="70"/>
-      <c r="J15" s="70"/>
-      <c r="K15" s="71"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="68"/>
+      <c r="K15" s="69"/>
     </row>
     <row r="16" spans="1:18" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="s">
@@ -1334,10 +1332,10 @@
       <c r="E16" s="17"/>
       <c r="F16" s="18"/>
       <c r="G16" s="26"/>
-      <c r="H16" s="70"/>
-      <c r="I16" s="70"/>
-      <c r="J16" s="70"/>
-      <c r="K16" s="71"/>
+      <c r="H16" s="68"/>
+      <c r="I16" s="68"/>
+      <c r="J16" s="68"/>
+      <c r="K16" s="69"/>
     </row>
     <row r="17" spans="1:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
@@ -1349,10 +1347,10 @@
       <c r="E17" s="17"/>
       <c r="F17" s="18"/>
       <c r="G17" s="26"/>
-      <c r="H17" s="70"/>
-      <c r="I17" s="70"/>
-      <c r="J17" s="70"/>
-      <c r="K17" s="71"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="68"/>
+      <c r="K17" s="69"/>
     </row>
     <row r="18" spans="1:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
@@ -1379,12 +1377,12 @@
       <c r="E19" s="17"/>
       <c r="F19" s="18"/>
       <c r="G19" s="7"/>
-      <c r="H19" s="72" t="str">
+      <c r="H19" s="70" t="str">
         <f>"BU ZARFTA "&amp;TEXT(Q9,"gg.aa.yyyy")&amp;" TARİHLİ UZLAŞMA TEKLİF FORMU VARDIR."</f>
         <v>BU ZARFTA 00.01.1900 TARİHLİ UZLAŞMA TEKLİF FORMU VARDIR.</v>
       </c>
-      <c r="I19" s="73"/>
-      <c r="J19" s="73"/>
+      <c r="I19" s="71"/>
+      <c r="J19" s="71"/>
       <c r="K19" s="28"/>
     </row>
     <row r="20" spans="1:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1397,9 +1395,9 @@
       <c r="E20" s="17"/>
       <c r="F20" s="18"/>
       <c r="G20" s="17"/>
-      <c r="H20" s="73"/>
-      <c r="I20" s="73"/>
-      <c r="J20" s="73"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="71"/>
+      <c r="J20" s="71"/>
       <c r="K20" s="18"/>
     </row>
     <row r="21" spans="1:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1414,9 +1412,9 @@
       </c>
       <c r="F21" s="20"/>
       <c r="G21" s="17"/>
-      <c r="H21" s="73"/>
-      <c r="I21" s="73"/>
-      <c r="J21" s="73"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="71"/>
+      <c r="J21" s="71"/>
       <c r="K21" s="18"/>
     </row>
     <row r="22" spans="1:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1431,9 +1429,9 @@
       </c>
       <c r="F22" s="20"/>
       <c r="G22" s="17"/>
-      <c r="H22" s="73"/>
-      <c r="I22" s="73"/>
-      <c r="J22" s="73"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="71"/>
+      <c r="J22" s="71"/>
       <c r="K22" s="18"/>
     </row>
     <row r="23" spans="1:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1535,13 +1533,13 @@
       <c r="K29" s="7"/>
     </row>
     <row r="30" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="64" t="s">
+      <c r="A30" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B30" s="65"/>
-      <c r="C30" s="65"/>
-      <c r="D30" s="65"/>
-      <c r="E30" s="65"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
       <c r="F30" s="39"/>
       <c r="G30" s="39"/>
       <c r="H30" s="39"/>
@@ -1550,41 +1548,42 @@
       <c r="K30" s="40"/>
     </row>
     <row r="31" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="58" t="s">
+      <c r="A31" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="59"/>
-      <c r="C31" s="59"/>
-      <c r="D31" s="59"/>
-      <c r="E31" s="59"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="57"/>
       <c r="F31" s="7"/>
-      <c r="G31" s="60" t="s">
+      <c r="G31" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="H31" s="61">
+      <c r="H31" s="59">
         <f>J2</f>
         <v>43435</v>
       </c>
-      <c r="I31" s="61"/>
-      <c r="J31" s="61" t="s">
-        <v>32</v>
-      </c>
-      <c r="K31" s="62"/>
+      <c r="I31" s="59"/>
+      <c r="J31" s="59">
+        <f>Q10</f>
+        <v>0</v>
+      </c>
+      <c r="K31" s="60"/>
     </row>
     <row r="32" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="58" t="s">
+      <c r="A32" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="59"/>
-      <c r="C32" s="59"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="59"/>
+      <c r="B32" s="57"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="57"/>
       <c r="F32" s="7"/>
-      <c r="G32" s="60"/>
-      <c r="H32" s="61"/>
-      <c r="I32" s="61"/>
-      <c r="J32" s="61"/>
-      <c r="K32" s="62"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="59"/>
+      <c r="I32" s="59"/>
+      <c r="J32" s="59"/>
+      <c r="K32" s="60"/>
     </row>
     <row r="33" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5"/>
@@ -1619,10 +1618,10 @@
       <c r="D35" s="17"/>
       <c r="E35" s="9"/>
       <c r="F35" s="17"/>
-      <c r="G35" s="63" t="s">
+      <c r="G35" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="H35" s="63"/>
+      <c r="H35" s="65"/>
       <c r="I35" s="17"/>
       <c r="J35" s="17"/>
       <c r="K35" s="18"/>
@@ -1634,8 +1633,8 @@
       <c r="D36" s="17"/>
       <c r="E36" s="9"/>
       <c r="F36" s="17"/>
-      <c r="G36" s="63"/>
-      <c r="H36" s="63"/>
+      <c r="G36" s="65"/>
+      <c r="H36" s="65"/>
       <c r="I36" s="17"/>
       <c r="J36" s="17"/>
       <c r="K36" s="18"/>
@@ -1680,14 +1679,14 @@
       <c r="K39" s="18"/>
     </row>
     <row r="40" spans="1:11" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="54" t="s">
+      <c r="A40" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="B40" s="55" t="str">
+      <c r="B40" s="67" t="str">
         <f>H10</f>
         <v>MEHMET EROĞLU</v>
       </c>
-      <c r="C40" s="55"/>
+      <c r="C40" s="67"/>
       <c r="D40" s="43"/>
       <c r="E40" s="43"/>
       <c r="F40" s="17"/>
@@ -1698,19 +1697,19 @@
       <c r="K40" s="18"/>
     </row>
     <row r="41" spans="1:11" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="54"/>
-      <c r="B41" s="55"/>
-      <c r="C41" s="55"/>
+      <c r="A41" s="66"/>
+      <c r="B41" s="67"/>
+      <c r="C41" s="67"/>
       <c r="D41" s="43"/>
       <c r="E41" s="43"/>
       <c r="F41" s="17"/>
       <c r="G41" s="26"/>
-      <c r="H41" s="56" t="str">
+      <c r="H41" s="72" t="str">
         <f>H19</f>
         <v>BU ZARFTA 00.01.1900 TARİHLİ UZLAŞMA TEKLİF FORMU VARDIR.</v>
       </c>
-      <c r="I41" s="56"/>
-      <c r="J41" s="56"/>
+      <c r="I41" s="72"/>
+      <c r="J41" s="72"/>
       <c r="K41" s="18"/>
     </row>
     <row r="42" spans="1:11" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1724,9 +1723,9 @@
       <c r="E42" s="45"/>
       <c r="F42" s="7"/>
       <c r="G42" s="26"/>
-      <c r="H42" s="56"/>
-      <c r="I42" s="56"/>
-      <c r="J42" s="56"/>
+      <c r="H42" s="72"/>
+      <c r="I42" s="72"/>
+      <c r="J42" s="72"/>
       <c r="K42" s="20"/>
     </row>
     <row r="43" spans="1:11" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1740,9 +1739,9 @@
       <c r="E43" s="45"/>
       <c r="F43" s="17"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="56"/>
-      <c r="I43" s="56"/>
-      <c r="J43" s="56"/>
+      <c r="H43" s="72"/>
+      <c r="I43" s="72"/>
+      <c r="J43" s="72"/>
       <c r="K43" s="20"/>
     </row>
     <row r="44" spans="1:11" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1753,22 +1752,22 @@
       <c r="E44" s="47"/>
       <c r="F44" s="43"/>
       <c r="G44" s="7"/>
-      <c r="H44" s="56"/>
-      <c r="I44" s="56"/>
-      <c r="J44" s="56"/>
+      <c r="H44" s="72"/>
+      <c r="I44" s="72"/>
+      <c r="J44" s="72"/>
       <c r="K44" s="48"/>
     </row>
     <row r="45" spans="1:11" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B45" s="57" t="str">
+      <c r="B45" s="73" t="str">
         <f>H15</f>
         <v>Ambarlı Mah Etinabk Tesisler Yolu Cad. Batman Apt. No:18 Daire 12 Avcılar İstanbul</v>
       </c>
-      <c r="C45" s="57"/>
-      <c r="D45" s="57"/>
-      <c r="E45" s="57"/>
+      <c r="C45" s="73"/>
+      <c r="D45" s="73"/>
+      <c r="E45" s="73"/>
       <c r="F45" s="43"/>
       <c r="G45" s="32"/>
       <c r="H45" s="17"/>
@@ -1778,10 +1777,10 @@
     </row>
     <row r="46" spans="1:11" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="46"/>
-      <c r="B46" s="57"/>
-      <c r="C46" s="57"/>
-      <c r="D46" s="57"/>
-      <c r="E46" s="57"/>
+      <c r="B46" s="73"/>
+      <c r="C46" s="73"/>
+      <c r="D46" s="73"/>
+      <c r="E46" s="73"/>
       <c r="F46" s="43"/>
       <c r="G46" s="32"/>
       <c r="H46" s="17"/>
@@ -1791,10 +1790,10 @@
     </row>
     <row r="47" spans="1:11" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="21"/>
-      <c r="B47" s="57"/>
-      <c r="C47" s="57"/>
-      <c r="D47" s="57"/>
-      <c r="E47" s="57"/>
+      <c r="B47" s="73"/>
+      <c r="C47" s="73"/>
+      <c r="D47" s="73"/>
+      <c r="E47" s="73"/>
       <c r="F47" s="43"/>
       <c r="G47" s="32"/>
       <c r="H47" s="17"/>
@@ -1923,6 +1922,16 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:C41"/>
+    <mergeCell ref="H41:J44"/>
+    <mergeCell ref="B45:E47"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="H31:I32"/>
+    <mergeCell ref="J31:K32"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="G35:H36"/>
     <mergeCell ref="A30:E30"/>
     <mergeCell ref="D1:H1"/>
     <mergeCell ref="D2:H2"/>
@@ -1935,16 +1944,6 @@
     <mergeCell ref="H10:I11"/>
     <mergeCell ref="H15:K17"/>
     <mergeCell ref="H19:J22"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:C41"/>
-    <mergeCell ref="H41:J44"/>
-    <mergeCell ref="B45:E47"/>
-    <mergeCell ref="A31:E31"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="H31:I32"/>
-    <mergeCell ref="J31:K32"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="G35:H36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>